<commit_message>
Fixed sort issue with table autofilters
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
@@ -10,6 +10,7 @@
     <x:sheet name="Single Column Strings" sheetId="3" r:id="rId3"/>
     <x:sheet name="Single Column Mixed" sheetId="4" r:id="rId4"/>
     <x:sheet name="Multi Column" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Table" sheetId="6" r:id="rId6"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Single Column Numbers'!$A$1:$A$7</x:definedName>
@@ -109,6 +110,24 @@
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
 </x:styleSheet>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A8" totalsRowCount="1">
+  <x:autoFilter ref="A1:A7">
+    <x:filterColumn colId="0">
+      <x:filters>
+        <x:filter val="3"/>
+        <x:filter val="4"/>
+        <x:filter val="5"/>
+      </x:filters>
+    </x:filterColumn>
+  </x:autoFilter>
+  <x:tableColumns count="1">
+    <x:tableColumn id="1" name="Numbers" totalsRowFunction="sum"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
@@ -707,4 +726,84 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A14"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="0" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:1">
+      <x:c r="A2" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:1">
+      <x:c r="A3" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:1">
+      <x:c r="A4" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:1">
+      <x:c r="A5" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:1" hidden="1">
+      <x:c r="A6" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:1" hidden="1">
+      <x:c r="A7" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:1">
+      <x:c r="A8" s="0">
+        <x:f>SUBTOTAL(109,[Numbers])</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:1">
+      <x:c r="A9" s="0" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:1">
+      <x:c r="A10" s="0" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:1">
+      <x:c r="A11" s="0" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:1">
+      <x:c r="A12" s="0" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:1">
+      <x:c r="A13" s="0" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:1">
+      <x:c r="A14" s="0" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="1">
+    <x:tablePart r:id="rId1"/>
+  </x:tableParts>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Misc bug fixes Added namedRange.RefersTo setter and namedRange.SetRefersTo(...) methods
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
@@ -733,7 +733,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A14"/>
+  <x:dimension ref="A1:A8"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -778,24 +778,6 @@
       <x:c r="A8" s="0">
         <x:f>SUBTOTAL(109,[Numbers])</x:f>
       </x:c>
-    </x:row>
-    <x:row r="9" spans="1:1">
-      <x:c r="A9" s="0" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:1">
-      <x:c r="A10" s="0" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:1">
-      <x:c r="A11" s="0" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:1">
-      <x:c r="A12" s="0" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:1">
-      <x:c r="A13" s="0" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:1">
-      <x:c r="A14" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>